<commit_message>
Atualização da resolução do Desafio 02
</commit_message>
<xml_diff>
--- a/bot-monitora-precos-site/precos.xlsx
+++ b/bot-monitora-precos-site/precos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Preço</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -454,6 +459,7 @@
       <c r="B2" t="n">
         <v>4.31004</v>
       </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -464,6 +470,7 @@
       <c r="B3" t="n">
         <v>4310.04</v>
       </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -473,6 +480,22 @@
       </c>
       <c r="B4" t="n">
         <v>4310.04</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4310.04</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Apple iPhone 14 (128 GB) – Meia-Noite</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>